<commit_message>
feat: mass spectrometry data support (#18)
* feat: add data entity for mass spectrometry

* chore: regen

* fix: typo in description

* refactor: consistent slot naming

* chore: regen

* chore: regen
</commit_message>
<xml_diff>
--- a/project/excel/modos_schema.xlsx
+++ b/project/excel/modos_schema.xlsx
@@ -16,8 +16,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Array" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODOCollection" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MassSpectrometryResults" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Array" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODOCollection" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -507,7 +508,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -520,6 +521,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>data_path</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data_format</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_sample</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -602,7 +664,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,15 +690,20 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>sample_processing</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -772,7 +839,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -945,7 +1012,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1006,7 +1073,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: add hash slot to DataEntity
</commit_message>
<xml_diff>
--- a/project/excel/modos_schema.xlsx
+++ b/project/excel/modos_schema.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODO" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assay" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sample" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MassSpectrometryResults" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Array" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODOCollection" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MODO" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Assay" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sample" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="MassSpectrometryResults" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Array" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="MODOCollection" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,15 +491,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -521,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,15 +557,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -791,7 +801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -822,15 +832,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -964,7 +979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,15 +1010,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1025,7 +1045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1056,15 +1076,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
feat: add hash slot to DataEntity (#21)
</commit_message>
<xml_diff>
--- a/project/excel/modos_schema.xlsx
+++ b/project/excel/modos_schema.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODO" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assay" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sample" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MassSpectrometryResults" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Array" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODOCollection" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MODO" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Assay" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sample" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="MassSpectrometryResults" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Array" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="MODOCollection" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,15 +491,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -521,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,15 +557,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -791,7 +801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -822,15 +832,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -964,7 +979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,15 +1010,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1025,7 +1045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1056,15 +1076,20 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>data_checksum</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
feat: add json and tsv to data formats
</commit_message>
<xml_diff>
--- a/project/excel/modos_schema.xlsx
+++ b/project/excel/modos_schema.xlsx
@@ -513,7 +513,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -579,7 +579,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -854,7 +854,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1032,7 +1032,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1098,7 +1098,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: json and tsv format support (#26)
* feat: add json and tsv to data formats
</commit_message>
<xml_diff>
--- a/project/excel/modos_schema.xlsx
+++ b/project/excel/modos_schema.xlsx
@@ -513,7 +513,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -579,7 +579,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -854,7 +854,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1032,7 +1032,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1098,7 +1098,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF,mzTab,TSV,JSON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
chore: python 3.13 support (#27)
* chore: bump dependencies

* chore: regen

* chore: bump version

* chore: regen

* ci: run on py313
</commit_message>
<xml_diff>
--- a/project/excel/modos_schema.xlsx
+++ b/project/excel/modos_schema.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="MODO" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Assay" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Sample" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="MassSpectrometryResults" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Array" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="MODOCollection" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODO" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assay" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sample" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MassSpectrometryResults" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Array" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODOCollection" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
feat: sample source_uri (#28)
* chore: make setup was run

* chore: regen
</commit_message>
<xml_diff>
--- a/project/excel/modos_schema.xlsx
+++ b/project/excel/modos_schema.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODO" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assay" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sample" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MassSpectrometryResults" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Array" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODOCollection" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MODO" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Assay" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sample" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="MassSpectrometryResults" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Array" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="MODOCollection" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -735,7 +735,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -771,15 +771,20 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>source_uri</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>